<commit_message>
Update BOC USD rates (auto)
</commit_message>
<xml_diff>
--- a/data/2026/2026-01.xlsx
+++ b/data/2026/2026-01.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,6 +613,58 @@
         </is>
       </c>
       <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.bankofchina.com/sourcedb/whpj/enindex_1619.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-02</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-02 17:53:08</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>697.85</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>697.85</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>700.79</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>700.79</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>702.88</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2026/01/02 17:53:08</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2026-01-02 09:56:30</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>https://www.bankofchina.com/sourcedb/whpj/enindex_1619.html</t>
         </is>
@@ -757,7 +809,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>